<commit_message>
Storage: simple cyclic SoC - Formulation adapted from PyPSA - Lack of high VRE nullifies storage - Constant import price nullifies storage
</commit_message>
<xml_diff>
--- a/data/zenodo/conversion/chp/CHE_convchp_biogas.xlsx
+++ b/data/zenodo/conversion/chp/CHE_convchp_biogas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/zenodo_ivan/conversion/chp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/zenodo/conversion/chp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BDD0F2-9748-D443-BD5D-5F8B67E309D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5AA554-19C4-3949-B09F-A828EC553A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$L$852</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$L$853</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2128" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="87">
   <si>
     <t>Name:</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>Maximum energy production per capacity unit, per year.</t>
+  </si>
+  <si>
+    <t>enable_year</t>
   </si>
 </sst>
 </file>
@@ -712,11 +715,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L432"/>
+  <dimension ref="A1:L433"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12:L12"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -820,16 +823,13 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>1990</v>
       </c>
       <c r="K7" s="2"/>
     </row>
@@ -841,13 +841,13 @@
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
         <v>83</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -862,19 +862,16 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G9">
-        <v>0.24</v>
-      </c>
-      <c r="J9" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="K9" s="2"/>
     </row>
@@ -886,16 +883,16 @@
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
         <v>79</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10">
-        <v>0.95</v>
+        <v>0.24</v>
       </c>
       <c r="J10" t="s">
         <v>46</v>
@@ -910,26 +907,21 @@
         <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>79</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
       </c>
       <c r="G11">
-        <v>0.25</v>
-      </c>
-      <c r="H11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" t="s">
-        <v>49</v>
+        <v>0.95</v>
       </c>
       <c r="J11" t="s">
         <v>46</v>
       </c>
-      <c r="L11" t="s">
-        <v>47</v>
-      </c>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -939,19 +931,25 @@
         <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
         <v>38</v>
       </c>
       <c r="G12">
-        <v>31.54</v>
+        <v>0.25</v>
       </c>
       <c r="H12" t="s">
-        <v>84</v>
+        <v>48</v>
+      </c>
+      <c r="I12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" t="s">
+        <v>46</v>
       </c>
       <c r="L12" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -961,25 +959,21 @@
       <c r="B13" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
+      <c r="C13" t="s">
+        <v>80</v>
       </c>
       <c r="D13" t="s">
         <v>38</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>31.54</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13" t="s">
-        <v>49</v>
-      </c>
-      <c r="J13" t="s">
-        <v>46</v>
-      </c>
-      <c r="K13" s="2"/>
+        <v>84</v>
+      </c>
+      <c r="L13" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -989,13 +983,16 @@
         <v>41</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
         <v>38</v>
       </c>
       <c r="G14">
-        <v>8.3000000000000007</v>
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>50</v>
       </c>
       <c r="I14" t="s">
         <v>49</v>
@@ -1013,23 +1010,21 @@
         <v>41</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
         <v>38</v>
       </c>
       <c r="G15">
-        <v>15</v>
-      </c>
-      <c r="H15" t="s">
-        <v>51</v>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I15" t="s">
+        <v>49</v>
       </c>
       <c r="J15" t="s">
-        <v>52</v>
-      </c>
-      <c r="L15" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1039,25 +1034,22 @@
         <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
         <v>38</v>
       </c>
       <c r="G16">
-        <v>2.66</v>
+        <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1068,21 +1060,26 @@
         <v>41</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
         <v>38</v>
       </c>
       <c r="G17">
-        <v>200</v>
+        <v>2.66</v>
       </c>
       <c r="H17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I17" t="s">
         <v>49</v>
       </c>
-      <c r="K17" s="2"/>
+      <c r="J17" t="s">
+        <v>55</v>
+      </c>
+      <c r="L17" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -1092,23 +1089,21 @@
         <v>41</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
         <v>38</v>
       </c>
       <c r="G18">
-        <v>0.88</v>
+        <v>200</v>
+      </c>
+      <c r="H18" t="s">
+        <v>57</v>
       </c>
       <c r="I18" t="s">
         <v>49</v>
       </c>
-      <c r="J18" t="s">
-        <v>58</v>
-      </c>
-      <c r="L18" t="s">
-        <v>59</v>
-      </c>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1118,22 +1113,22 @@
         <v>41</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
         <v>38</v>
       </c>
       <c r="G19">
-        <v>0.6</v>
+        <v>0.88</v>
       </c>
       <c r="I19" t="s">
         <v>49</v>
       </c>
       <c r="J19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1143,32 +1138,23 @@
       <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="C20" t="s">
-        <v>17</v>
+      <c r="C20" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20">
-        <v>1990</v>
+        <v>38</v>
       </c>
       <c r="G20">
-        <v>80</v>
-      </c>
-      <c r="H20" t="s">
-        <v>62</v>
+        <v>0.6</v>
       </c>
       <c r="I20" t="s">
         <v>49</v>
       </c>
       <c r="J20" t="s">
-        <v>63</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1185,10 +1171,10 @@
         <v>39</v>
       </c>
       <c r="E21">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G21">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H21" t="s">
         <v>62</v>
@@ -1220,10 +1206,10 @@
         <v>39</v>
       </c>
       <c r="E22">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G22">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="H22" t="s">
         <v>62</v>
@@ -1255,10 +1241,10 @@
         <v>39</v>
       </c>
       <c r="E23">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G23">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="H23" t="s">
         <v>62</v>
@@ -1290,10 +1276,10 @@
         <v>39</v>
       </c>
       <c r="E24">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G24">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="H24" t="s">
         <v>62</v>
@@ -1325,10 +1311,10 @@
         <v>39</v>
       </c>
       <c r="E25">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G25">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H25" t="s">
         <v>62</v>
@@ -1360,10 +1346,10 @@
         <v>39</v>
       </c>
       <c r="E26">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G26">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H26" t="s">
         <v>62</v>
@@ -1395,10 +1381,10 @@
         <v>39</v>
       </c>
       <c r="E27">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G27">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H27" t="s">
         <v>62</v>
@@ -1430,10 +1416,10 @@
         <v>39</v>
       </c>
       <c r="E28">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G28">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="H28" t="s">
         <v>62</v>
@@ -1465,10 +1451,10 @@
         <v>39</v>
       </c>
       <c r="E29">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G29">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="H29" t="s">
         <v>62</v>
@@ -1500,10 +1486,10 @@
         <v>39</v>
       </c>
       <c r="E30">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G30">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="H30" t="s">
         <v>62</v>
@@ -1535,10 +1521,10 @@
         <v>39</v>
       </c>
       <c r="E31">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G31">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="H31" t="s">
         <v>62</v>
@@ -1570,10 +1556,10 @@
         <v>39</v>
       </c>
       <c r="E32">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G32">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="H32" t="s">
         <v>62</v>
@@ -1605,10 +1591,10 @@
         <v>39</v>
       </c>
       <c r="E33">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G33">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H33" t="s">
         <v>62</v>
@@ -1640,10 +1626,10 @@
         <v>39</v>
       </c>
       <c r="E34">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G34">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H34" t="s">
         <v>62</v>
@@ -1675,10 +1661,10 @@
         <v>39</v>
       </c>
       <c r="E35">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G35">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H35" t="s">
         <v>62</v>
@@ -1710,10 +1696,10 @@
         <v>39</v>
       </c>
       <c r="E36">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G36">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="H36" t="s">
         <v>62</v>
@@ -1745,10 +1731,10 @@
         <v>39</v>
       </c>
       <c r="E37">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G37">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="H37" t="s">
         <v>62</v>
@@ -1780,10 +1766,10 @@
         <v>39</v>
       </c>
       <c r="E38">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G38">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H38" t="s">
         <v>62</v>
@@ -1815,10 +1801,10 @@
         <v>39</v>
       </c>
       <c r="E39">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G39">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="H39" t="s">
         <v>62</v>
@@ -1850,10 +1836,10 @@
         <v>39</v>
       </c>
       <c r="E40">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G40">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="H40" t="s">
         <v>62</v>
@@ -1885,10 +1871,10 @@
         <v>39</v>
       </c>
       <c r="E41">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G41">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="H41" t="s">
         <v>62</v>
@@ -1920,10 +1906,10 @@
         <v>39</v>
       </c>
       <c r="E42">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G42">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="H42" t="s">
         <v>62</v>
@@ -1955,10 +1941,10 @@
         <v>39</v>
       </c>
       <c r="E43">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G43">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="H43" t="s">
         <v>62</v>
@@ -1990,10 +1976,10 @@
         <v>39</v>
       </c>
       <c r="E44">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G44">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="H44" t="s">
         <v>62</v>
@@ -2025,10 +2011,10 @@
         <v>39</v>
       </c>
       <c r="E45">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G45">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="H45" t="s">
         <v>62</v>
@@ -2060,10 +2046,10 @@
         <v>39</v>
       </c>
       <c r="E46">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G46">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="H46" t="s">
         <v>62</v>
@@ -2095,10 +2081,10 @@
         <v>39</v>
       </c>
       <c r="E47">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G47">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="H47" t="s">
         <v>62</v>
@@ -2130,10 +2116,10 @@
         <v>39</v>
       </c>
       <c r="E48">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G48">
-        <v>352</v>
+        <v>334</v>
       </c>
       <c r="H48" t="s">
         <v>62</v>
@@ -2165,10 +2151,10 @@
         <v>39</v>
       </c>
       <c r="E49">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G49">
-        <v>372</v>
+        <v>352</v>
       </c>
       <c r="H49" t="s">
         <v>62</v>
@@ -2194,31 +2180,31 @@
         <v>41</v>
       </c>
       <c r="C50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D50" t="s">
         <v>39</v>
       </c>
       <c r="E50">
-        <v>1990</v>
+        <v>2019</v>
       </c>
       <c r="G50">
-        <v>21.04945055</v>
+        <v>372</v>
       </c>
       <c r="H50" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="I50" t="s">
         <v>49</v>
       </c>
       <c r="J50" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L50" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -2235,10 +2221,10 @@
         <v>39</v>
       </c>
       <c r="E51">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G51">
-        <v>22.33894102</v>
+        <v>21.04945055</v>
       </c>
       <c r="H51" t="s">
         <v>57</v>
@@ -2270,10 +2256,10 @@
         <v>39</v>
       </c>
       <c r="E52">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G52">
-        <v>24.121794869999999</v>
+        <v>22.33894102</v>
       </c>
       <c r="H52" t="s">
         <v>57</v>
@@ -2305,10 +2291,10 @@
         <v>39</v>
       </c>
       <c r="E53">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G53">
-        <v>28.876117319999999</v>
+        <v>24.121794869999999</v>
       </c>
       <c r="H53" t="s">
         <v>57</v>
@@ -2340,10 +2326,10 @@
         <v>39</v>
       </c>
       <c r="E54">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G54">
-        <v>32.853846150000003</v>
+        <v>28.876117319999999</v>
       </c>
       <c r="H54" t="s">
         <v>57</v>
@@ -2375,10 +2361,10 @@
         <v>39</v>
       </c>
       <c r="E55">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G55">
-        <v>34.257856670000002</v>
+        <v>32.853846150000003</v>
       </c>
       <c r="H55" t="s">
         <v>57</v>
@@ -2410,10 +2396,10 @@
         <v>39</v>
       </c>
       <c r="E56">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G56">
-        <v>34.946620449999998</v>
+        <v>34.257856670000002</v>
       </c>
       <c r="H56" t="s">
         <v>57</v>
@@ -2445,10 +2431,10 @@
         <v>39</v>
       </c>
       <c r="E57">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G57">
-        <v>37.418197569999997</v>
+        <v>34.946620449999998</v>
       </c>
       <c r="H57" t="s">
         <v>57</v>
@@ -2480,10 +2466,10 @@
         <v>39</v>
       </c>
       <c r="E58">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G58">
-        <v>42.526392250000001</v>
+        <v>37.418197569999997</v>
       </c>
       <c r="H58" t="s">
         <v>57</v>
@@ -2515,7 +2501,7 @@
         <v>39</v>
       </c>
       <c r="E59">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G59">
         <v>42.526392250000001</v>
@@ -2550,7 +2536,7 @@
         <v>39</v>
       </c>
       <c r="E60">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G60">
         <v>42.526392250000001</v>
@@ -2585,10 +2571,10 @@
         <v>39</v>
       </c>
       <c r="E61">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G61">
-        <v>45.701244060000001</v>
+        <v>42.526392250000001</v>
       </c>
       <c r="H61" t="s">
         <v>57</v>
@@ -2620,10 +2606,10 @@
         <v>39</v>
       </c>
       <c r="E62">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G62">
-        <v>50.615668599999999</v>
+        <v>45.701244060000001</v>
       </c>
       <c r="H62" t="s">
         <v>57</v>
@@ -2655,7 +2641,7 @@
         <v>39</v>
       </c>
       <c r="E63">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G63">
         <v>50.615668599999999</v>
@@ -2690,10 +2676,10 @@
         <v>39</v>
       </c>
       <c r="E64">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G64">
-        <v>51.870777320000002</v>
+        <v>50.615668599999999</v>
       </c>
       <c r="H64" t="s">
         <v>57</v>
@@ -2725,7 +2711,7 @@
         <v>39</v>
       </c>
       <c r="E65">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G65">
         <v>51.870777320000002</v>
@@ -2760,10 +2746,10 @@
         <v>39</v>
       </c>
       <c r="E66">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G66">
-        <v>53.558998899999999</v>
+        <v>51.870777320000002</v>
       </c>
       <c r="H66" t="s">
         <v>57</v>
@@ -2795,7 +2781,7 @@
         <v>39</v>
       </c>
       <c r="E67">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G67">
         <v>53.558998899999999</v>
@@ -2830,7 +2816,7 @@
         <v>39</v>
       </c>
       <c r="E68">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G68">
         <v>53.558998899999999</v>
@@ -2865,7 +2851,7 @@
         <v>39</v>
       </c>
       <c r="E69">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G69">
         <v>53.558998899999999</v>
@@ -2900,7 +2886,7 @@
         <v>39</v>
       </c>
       <c r="E70">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G70">
         <v>53.558998899999999</v>
@@ -2935,7 +2921,7 @@
         <v>39</v>
       </c>
       <c r="E71">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G71">
         <v>53.558998899999999</v>
@@ -2970,7 +2956,7 @@
         <v>39</v>
       </c>
       <c r="E72">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G72">
         <v>53.558998899999999</v>
@@ -3005,7 +2991,7 @@
         <v>39</v>
       </c>
       <c r="E73">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G73">
         <v>53.558998899999999</v>
@@ -3040,7 +3026,7 @@
         <v>39</v>
       </c>
       <c r="E74">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G74">
         <v>53.558998899999999</v>
@@ -3075,7 +3061,7 @@
         <v>39</v>
       </c>
       <c r="E75">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G75">
         <v>53.558998899999999</v>
@@ -3110,7 +3096,7 @@
         <v>39</v>
       </c>
       <c r="E76">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G76">
         <v>53.558998899999999</v>
@@ -3145,10 +3131,10 @@
         <v>39</v>
       </c>
       <c r="E77">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G77">
-        <v>56.087386670000001</v>
+        <v>53.558998899999999</v>
       </c>
       <c r="H77" t="s">
         <v>57</v>
@@ -3180,10 +3166,10 @@
         <v>39</v>
       </c>
       <c r="E78">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G78">
-        <v>60.844335350000001</v>
+        <v>56.087386670000001</v>
       </c>
       <c r="H78" t="s">
         <v>57</v>
@@ -3215,7 +3201,7 @@
         <v>39</v>
       </c>
       <c r="E79">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G79">
         <v>60.844335350000001</v>
@@ -3244,16 +3230,16 @@
         <v>41</v>
       </c>
       <c r="C80" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D80" t="s">
         <v>39</v>
       </c>
       <c r="E80">
-        <v>1990</v>
+        <v>2019</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>60.844335350000001</v>
       </c>
       <c r="H80" t="s">
         <v>57</v>
@@ -3264,8 +3250,11 @@
       <c r="J80" t="s">
         <v>66</v>
       </c>
+      <c r="K80" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="L80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
@@ -3282,10 +3271,10 @@
         <v>39</v>
       </c>
       <c r="E81">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G81">
-        <v>1.289490469</v>
+        <v>0</v>
       </c>
       <c r="H81" t="s">
         <v>57</v>
@@ -3314,10 +3303,10 @@
         <v>39</v>
       </c>
       <c r="E82">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G82">
-        <v>1.782853853</v>
+        <v>1.289490469</v>
       </c>
       <c r="H82" t="s">
         <v>57</v>
@@ -3346,10 +3335,10 @@
         <v>39</v>
       </c>
       <c r="E83">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G83">
-        <v>4.7543224469999998</v>
+        <v>1.782853853</v>
       </c>
       <c r="H83" t="s">
         <v>57</v>
@@ -3378,10 +3367,10 @@
         <v>39</v>
       </c>
       <c r="E84">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G84">
-        <v>3.9777288350000002</v>
+        <v>4.7543224469999998</v>
       </c>
       <c r="H84" t="s">
         <v>57</v>
@@ -3410,10 +3399,10 @@
         <v>39</v>
       </c>
       <c r="E85">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G85">
-        <v>1.4040105190000001</v>
+        <v>3.9777288350000002</v>
       </c>
       <c r="H85" t="s">
         <v>57</v>
@@ -3442,10 +3431,10 @@
         <v>39</v>
       </c>
       <c r="E86">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G86">
-        <v>0.68876377700000002</v>
+        <v>1.4040105190000001</v>
       </c>
       <c r="H86" t="s">
         <v>57</v>
@@ -3474,10 +3463,10 @@
         <v>39</v>
       </c>
       <c r="E87">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G87">
-        <v>2.4715771229999999</v>
+        <v>0.68876377700000002</v>
       </c>
       <c r="H87" t="s">
         <v>57</v>
@@ -3506,10 +3495,10 @@
         <v>39</v>
       </c>
       <c r="E88">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G88">
-        <v>5.1081946780000003</v>
+        <v>2.4715771229999999</v>
       </c>
       <c r="H88" t="s">
         <v>57</v>
@@ -3538,10 +3527,10 @@
         <v>39</v>
       </c>
       <c r="E89">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>5.1081946780000003</v>
       </c>
       <c r="H89" t="s">
         <v>57</v>
@@ -3570,7 +3559,7 @@
         <v>39</v>
       </c>
       <c r="E90">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -3602,10 +3591,10 @@
         <v>39</v>
       </c>
       <c r="E91">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G91">
-        <v>3.1748518040000002</v>
+        <v>0</v>
       </c>
       <c r="H91" t="s">
         <v>57</v>
@@ -3634,10 +3623,10 @@
         <v>39</v>
       </c>
       <c r="E92">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G92">
-        <v>4.9144245419999999</v>
+        <v>3.1748518040000002</v>
       </c>
       <c r="H92" t="s">
         <v>57</v>
@@ -3666,10 +3655,10 @@
         <v>39</v>
       </c>
       <c r="E93">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>4.9144245419999999</v>
       </c>
       <c r="H93" t="s">
         <v>57</v>
@@ -3698,10 +3687,10 @@
         <v>39</v>
       </c>
       <c r="E94">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G94">
-        <v>1.2551087249999999</v>
+        <v>0</v>
       </c>
       <c r="H94" t="s">
         <v>57</v>
@@ -3730,10 +3719,10 @@
         <v>39</v>
       </c>
       <c r="E95">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>1.2551087249999999</v>
       </c>
       <c r="H95" t="s">
         <v>57</v>
@@ -3762,10 +3751,10 @@
         <v>39</v>
       </c>
       <c r="E96">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G96">
-        <v>1.6882215780000001</v>
+        <v>0</v>
       </c>
       <c r="H96" t="s">
         <v>57</v>
@@ -3794,10 +3783,10 @@
         <v>39</v>
       </c>
       <c r="E97">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G97">
-        <v>0</v>
+        <v>1.6882215780000001</v>
       </c>
       <c r="H97" t="s">
         <v>57</v>
@@ -3826,7 +3815,7 @@
         <v>39</v>
       </c>
       <c r="E98">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -3858,7 +3847,7 @@
         <v>39</v>
       </c>
       <c r="E99">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -3890,7 +3879,7 @@
         <v>39</v>
       </c>
       <c r="E100">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -3922,7 +3911,7 @@
         <v>39</v>
       </c>
       <c r="E101">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -3954,7 +3943,7 @@
         <v>39</v>
       </c>
       <c r="E102">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -3986,7 +3975,7 @@
         <v>39</v>
       </c>
       <c r="E103">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -4018,7 +4007,7 @@
         <v>39</v>
       </c>
       <c r="E104">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -4050,7 +4039,7 @@
         <v>39</v>
       </c>
       <c r="E105">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -4082,7 +4071,7 @@
         <v>39</v>
       </c>
       <c r="E106">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -4114,10 +4103,10 @@
         <v>39</v>
       </c>
       <c r="E107">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G107">
-        <v>2.5283877709999998</v>
+        <v>0</v>
       </c>
       <c r="H107" t="s">
         <v>57</v>
@@ -4146,10 +4135,10 @@
         <v>39</v>
       </c>
       <c r="E108">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G108">
-        <v>4.756948682</v>
+        <v>2.5283877709999998</v>
       </c>
       <c r="H108" t="s">
         <v>57</v>
@@ -4178,10 +4167,10 @@
         <v>39</v>
       </c>
       <c r="E109">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G109">
-        <v>0</v>
+        <v>4.756948682</v>
       </c>
       <c r="H109" t="s">
         <v>57</v>
@@ -4204,13 +4193,13 @@
         <v>41</v>
       </c>
       <c r="C110" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D110" t="s">
         <v>39</v>
       </c>
       <c r="E110">
-        <v>1990</v>
+        <v>2019</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -4242,7 +4231,7 @@
         <v>39</v>
       </c>
       <c r="E111">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -4274,7 +4263,7 @@
         <v>39</v>
       </c>
       <c r="E112">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -4306,7 +4295,7 @@
         <v>39</v>
       </c>
       <c r="E113">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -4338,7 +4327,7 @@
         <v>39</v>
       </c>
       <c r="E114">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -4370,7 +4359,7 @@
         <v>39</v>
       </c>
       <c r="E115">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -4402,7 +4391,7 @@
         <v>39</v>
       </c>
       <c r="E116">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G116">
         <v>0</v>
@@ -4434,7 +4423,7 @@
         <v>39</v>
       </c>
       <c r="E117">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -4466,7 +4455,7 @@
         <v>39</v>
       </c>
       <c r="E118">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -4498,7 +4487,7 @@
         <v>39</v>
       </c>
       <c r="E119">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -4530,7 +4519,7 @@
         <v>39</v>
       </c>
       <c r="E120">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -4562,7 +4551,7 @@
         <v>39</v>
       </c>
       <c r="E121">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -4594,7 +4583,7 @@
         <v>39</v>
       </c>
       <c r="E122">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -4626,7 +4615,7 @@
         <v>39</v>
       </c>
       <c r="E123">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -4658,7 +4647,7 @@
         <v>39</v>
       </c>
       <c r="E124">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G124">
         <v>0</v>
@@ -4690,7 +4679,7 @@
         <v>39</v>
       </c>
       <c r="E125">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G125">
         <v>0</v>
@@ -4722,7 +4711,7 @@
         <v>39</v>
       </c>
       <c r="E126">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G126">
         <v>0</v>
@@ -4754,7 +4743,7 @@
         <v>39</v>
       </c>
       <c r="E127">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G127">
         <v>0</v>
@@ -4786,7 +4775,7 @@
         <v>39</v>
       </c>
       <c r="E128">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G128">
         <v>0</v>
@@ -4818,7 +4807,7 @@
         <v>39</v>
       </c>
       <c r="E129">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G129">
         <v>0</v>
@@ -4850,7 +4839,7 @@
         <v>39</v>
       </c>
       <c r="E130">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G130">
         <v>0</v>
@@ -4882,7 +4871,7 @@
         <v>39</v>
       </c>
       <c r="E131">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G131">
         <v>0</v>
@@ -4914,7 +4903,7 @@
         <v>39</v>
       </c>
       <c r="E132">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G132">
         <v>0</v>
@@ -4946,7 +4935,7 @@
         <v>39</v>
       </c>
       <c r="E133">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G133">
         <v>0</v>
@@ -4978,7 +4967,7 @@
         <v>39</v>
       </c>
       <c r="E134">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G134">
         <v>0</v>
@@ -5010,7 +4999,7 @@
         <v>39</v>
       </c>
       <c r="E135">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G135">
         <v>0</v>
@@ -5042,7 +5031,7 @@
         <v>39</v>
       </c>
       <c r="E136">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G136">
         <v>0</v>
@@ -5074,7 +5063,7 @@
         <v>39</v>
       </c>
       <c r="E137">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G137">
         <v>0</v>
@@ -5106,7 +5095,7 @@
         <v>39</v>
       </c>
       <c r="E138">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G138">
         <v>0</v>
@@ -5138,7 +5127,7 @@
         <v>39</v>
       </c>
       <c r="E139">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G139">
         <v>0</v>
@@ -5164,16 +5153,28 @@
         <v>41</v>
       </c>
       <c r="C140" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D140" t="s">
         <v>39</v>
       </c>
       <c r="E140">
-        <v>1990</v>
+        <v>2019</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+      <c r="H140" t="s">
+        <v>57</v>
       </c>
       <c r="I140" t="s">
         <v>49</v>
+      </c>
+      <c r="J140" t="s">
+        <v>66</v>
+      </c>
+      <c r="L140" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.2">
@@ -5190,7 +5191,7 @@
         <v>39</v>
       </c>
       <c r="E141">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="I141" t="s">
         <v>49</v>
@@ -5210,7 +5211,7 @@
         <v>39</v>
       </c>
       <c r="E142">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="I142" t="s">
         <v>49</v>
@@ -5230,7 +5231,7 @@
         <v>39</v>
       </c>
       <c r="E143">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="I143" t="s">
         <v>49</v>
@@ -5250,7 +5251,7 @@
         <v>39</v>
       </c>
       <c r="E144">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="I144" t="s">
         <v>49</v>
@@ -5270,7 +5271,7 @@
         <v>39</v>
       </c>
       <c r="E145">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="I145" t="s">
         <v>49</v>
@@ -5290,7 +5291,7 @@
         <v>39</v>
       </c>
       <c r="E146">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="I146" t="s">
         <v>49</v>
@@ -5310,7 +5311,7 @@
         <v>39</v>
       </c>
       <c r="E147">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="I147" t="s">
         <v>49</v>
@@ -5330,7 +5331,7 @@
         <v>39</v>
       </c>
       <c r="E148">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="I148" t="s">
         <v>49</v>
@@ -5350,7 +5351,7 @@
         <v>39</v>
       </c>
       <c r="E149">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="I149" t="s">
         <v>49</v>
@@ -5370,7 +5371,7 @@
         <v>39</v>
       </c>
       <c r="E150">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="I150" t="s">
         <v>49</v>
@@ -5390,7 +5391,7 @@
         <v>39</v>
       </c>
       <c r="E151">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="I151" t="s">
         <v>49</v>
@@ -5410,7 +5411,7 @@
         <v>39</v>
       </c>
       <c r="E152">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="I152" t="s">
         <v>49</v>
@@ -5430,7 +5431,7 @@
         <v>39</v>
       </c>
       <c r="E153">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="I153" t="s">
         <v>49</v>
@@ -5450,7 +5451,7 @@
         <v>39</v>
       </c>
       <c r="E154">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="I154" t="s">
         <v>49</v>
@@ -5470,7 +5471,7 @@
         <v>39</v>
       </c>
       <c r="E155">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="I155" t="s">
         <v>49</v>
@@ -5490,7 +5491,7 @@
         <v>39</v>
       </c>
       <c r="E156">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="I156" t="s">
         <v>49</v>
@@ -5510,7 +5511,7 @@
         <v>39</v>
       </c>
       <c r="E157">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="I157" t="s">
         <v>49</v>
@@ -5530,7 +5531,7 @@
         <v>39</v>
       </c>
       <c r="E158">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="I158" t="s">
         <v>49</v>
@@ -5550,7 +5551,7 @@
         <v>39</v>
       </c>
       <c r="E159">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="I159" t="s">
         <v>49</v>
@@ -5570,7 +5571,7 @@
         <v>39</v>
       </c>
       <c r="E160">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="I160" t="s">
         <v>49</v>
@@ -5590,7 +5591,7 @@
         <v>39</v>
       </c>
       <c r="E161">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="I161" t="s">
         <v>49</v>
@@ -5610,7 +5611,7 @@
         <v>39</v>
       </c>
       <c r="E162">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="I162" t="s">
         <v>49</v>
@@ -5630,7 +5631,7 @@
         <v>39</v>
       </c>
       <c r="E163">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="I163" t="s">
         <v>49</v>
@@ -5650,7 +5651,7 @@
         <v>39</v>
       </c>
       <c r="E164">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="I164" t="s">
         <v>49</v>
@@ -5670,7 +5671,7 @@
         <v>39</v>
       </c>
       <c r="E165">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="I165" t="s">
         <v>49</v>
@@ -5690,7 +5691,7 @@
         <v>39</v>
       </c>
       <c r="E166">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I166" t="s">
         <v>49</v>
@@ -5710,7 +5711,7 @@
         <v>39</v>
       </c>
       <c r="E167">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="I167" t="s">
         <v>49</v>
@@ -5730,22 +5731,10 @@
         <v>39</v>
       </c>
       <c r="E168">
-        <v>2018</v>
-      </c>
-      <c r="G168">
-        <v>538</v>
-      </c>
-      <c r="H168" t="s">
-        <v>70</v>
+        <v>2017</v>
       </c>
       <c r="I168" t="s">
         <v>49</v>
-      </c>
-      <c r="J168" t="s">
-        <v>52</v>
-      </c>
-      <c r="L168" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.2">
@@ -5762,10 +5751,22 @@
         <v>39</v>
       </c>
       <c r="E169">
-        <v>2019</v>
+        <v>2018</v>
+      </c>
+      <c r="G169">
+        <v>538</v>
+      </c>
+      <c r="H169" t="s">
+        <v>70</v>
       </c>
       <c r="I169" t="s">
         <v>49</v>
+      </c>
+      <c r="J169" t="s">
+        <v>52</v>
+      </c>
+      <c r="L169" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.2">
@@ -5776,13 +5777,13 @@
         <v>41</v>
       </c>
       <c r="C170" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D170" t="s">
         <v>39</v>
       </c>
       <c r="E170">
-        <v>1990</v>
+        <v>2019</v>
       </c>
       <c r="I170" t="s">
         <v>49</v>
@@ -5802,7 +5803,7 @@
         <v>39</v>
       </c>
       <c r="E171">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="I171" t="s">
         <v>49</v>
@@ -5822,7 +5823,7 @@
         <v>39</v>
       </c>
       <c r="E172">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="I172" t="s">
         <v>49</v>
@@ -5842,7 +5843,7 @@
         <v>39</v>
       </c>
       <c r="E173">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="I173" t="s">
         <v>49</v>
@@ -5862,7 +5863,7 @@
         <v>39</v>
       </c>
       <c r="E174">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="I174" t="s">
         <v>49</v>
@@ -5882,7 +5883,7 @@
         <v>39</v>
       </c>
       <c r="E175">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="I175" t="s">
         <v>49</v>
@@ -5902,7 +5903,7 @@
         <v>39</v>
       </c>
       <c r="E176">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="I176" t="s">
         <v>49</v>
@@ -5922,7 +5923,7 @@
         <v>39</v>
       </c>
       <c r="E177">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="I177" t="s">
         <v>49</v>
@@ -5942,7 +5943,7 @@
         <v>39</v>
       </c>
       <c r="E178">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="I178" t="s">
         <v>49</v>
@@ -5962,7 +5963,7 @@
         <v>39</v>
       </c>
       <c r="E179">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="I179" t="s">
         <v>49</v>
@@ -5982,7 +5983,7 @@
         <v>39</v>
       </c>
       <c r="E180">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="I180" t="s">
         <v>49</v>
@@ -6002,7 +6003,7 @@
         <v>39</v>
       </c>
       <c r="E181">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="I181" t="s">
         <v>49</v>
@@ -6022,7 +6023,7 @@
         <v>39</v>
       </c>
       <c r="E182">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="I182" t="s">
         <v>49</v>
@@ -6042,7 +6043,7 @@
         <v>39</v>
       </c>
       <c r="E183">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="I183" t="s">
         <v>49</v>
@@ -6062,7 +6063,7 @@
         <v>39</v>
       </c>
       <c r="E184">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="I184" t="s">
         <v>49</v>
@@ -6082,7 +6083,7 @@
         <v>39</v>
       </c>
       <c r="E185">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="I185" t="s">
         <v>49</v>
@@ -6102,7 +6103,7 @@
         <v>39</v>
       </c>
       <c r="E186">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="I186" t="s">
         <v>49</v>
@@ -6122,7 +6123,7 @@
         <v>39</v>
       </c>
       <c r="E187">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="I187" t="s">
         <v>49</v>
@@ -6142,7 +6143,7 @@
         <v>39</v>
       </c>
       <c r="E188">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="I188" t="s">
         <v>49</v>
@@ -6162,7 +6163,7 @@
         <v>39</v>
       </c>
       <c r="E189">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="I189" t="s">
         <v>49</v>
@@ -6182,7 +6183,7 @@
         <v>39</v>
       </c>
       <c r="E190">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="I190" t="s">
         <v>49</v>
@@ -6202,7 +6203,7 @@
         <v>39</v>
       </c>
       <c r="E191">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="I191" t="s">
         <v>49</v>
@@ -6222,7 +6223,7 @@
         <v>39</v>
       </c>
       <c r="E192">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="I192" t="s">
         <v>49</v>
@@ -6242,7 +6243,7 @@
         <v>39</v>
       </c>
       <c r="E193">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="I193" t="s">
         <v>49</v>
@@ -6262,7 +6263,7 @@
         <v>39</v>
       </c>
       <c r="E194">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="I194" t="s">
         <v>49</v>
@@ -6282,7 +6283,7 @@
         <v>39</v>
       </c>
       <c r="E195">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="I195" t="s">
         <v>49</v>
@@ -6302,7 +6303,7 @@
         <v>39</v>
       </c>
       <c r="E196">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I196" t="s">
         <v>49</v>
@@ -6322,7 +6323,7 @@
         <v>39</v>
       </c>
       <c r="E197">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="I197" t="s">
         <v>49</v>
@@ -6342,22 +6343,10 @@
         <v>39</v>
       </c>
       <c r="E198">
-        <v>2018</v>
-      </c>
-      <c r="G198">
-        <v>9532</v>
-      </c>
-      <c r="H198" t="s">
-        <v>70</v>
+        <v>2017</v>
       </c>
       <c r="I198" t="s">
         <v>49</v>
-      </c>
-      <c r="J198" t="s">
-        <v>52</v>
-      </c>
-      <c r="L198" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.2">
@@ -6374,10 +6363,22 @@
         <v>39</v>
       </c>
       <c r="E199">
-        <v>2019</v>
+        <v>2018</v>
+      </c>
+      <c r="G199">
+        <v>9532</v>
+      </c>
+      <c r="H199" t="s">
+        <v>70</v>
       </c>
       <c r="I199" t="s">
         <v>49</v>
+      </c>
+      <c r="J199" t="s">
+        <v>52</v>
+      </c>
+      <c r="L199" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.2">
@@ -6388,13 +6389,13 @@
         <v>41</v>
       </c>
       <c r="C200" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D200" t="s">
         <v>39</v>
       </c>
       <c r="E200">
-        <v>1990</v>
+        <v>2019</v>
       </c>
       <c r="I200" t="s">
         <v>49</v>
@@ -6414,7 +6415,7 @@
         <v>39</v>
       </c>
       <c r="E201">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="I201" t="s">
         <v>49</v>
@@ -6434,7 +6435,7 @@
         <v>39</v>
       </c>
       <c r="E202">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="I202" t="s">
         <v>49</v>
@@ -6454,7 +6455,7 @@
         <v>39</v>
       </c>
       <c r="E203">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="I203" t="s">
         <v>49</v>
@@ -6474,7 +6475,7 @@
         <v>39</v>
       </c>
       <c r="E204">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="I204" t="s">
         <v>49</v>
@@ -6494,7 +6495,7 @@
         <v>39</v>
       </c>
       <c r="E205">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="I205" t="s">
         <v>49</v>
@@ -6514,7 +6515,7 @@
         <v>39</v>
       </c>
       <c r="E206">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="I206" t="s">
         <v>49</v>
@@ -6534,7 +6535,7 @@
         <v>39</v>
       </c>
       <c r="E207">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="I207" t="s">
         <v>49</v>
@@ -6554,7 +6555,7 @@
         <v>39</v>
       </c>
       <c r="E208">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="I208" t="s">
         <v>49</v>
@@ -6574,7 +6575,7 @@
         <v>39</v>
       </c>
       <c r="E209">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="I209" t="s">
         <v>49</v>
@@ -6594,7 +6595,7 @@
         <v>39</v>
       </c>
       <c r="E210">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="I210" t="s">
         <v>49</v>
@@ -6614,7 +6615,7 @@
         <v>39</v>
       </c>
       <c r="E211">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="I211" t="s">
         <v>49</v>
@@ -6634,7 +6635,7 @@
         <v>39</v>
       </c>
       <c r="E212">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="I212" t="s">
         <v>49</v>
@@ -6654,7 +6655,7 @@
         <v>39</v>
       </c>
       <c r="E213">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="I213" t="s">
         <v>49</v>
@@ -6674,7 +6675,7 @@
         <v>39</v>
       </c>
       <c r="E214">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="I214" t="s">
         <v>49</v>
@@ -6694,7 +6695,7 @@
         <v>39</v>
       </c>
       <c r="E215">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="I215" t="s">
         <v>49</v>
@@ -6714,7 +6715,7 @@
         <v>39</v>
       </c>
       <c r="E216">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="I216" t="s">
         <v>49</v>
@@ -6734,7 +6735,7 @@
         <v>39</v>
       </c>
       <c r="E217">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="I217" t="s">
         <v>49</v>
@@ -6754,7 +6755,7 @@
         <v>39</v>
       </c>
       <c r="E218">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="I218" t="s">
         <v>49</v>
@@ -6774,7 +6775,7 @@
         <v>39</v>
       </c>
       <c r="E219">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="I219" t="s">
         <v>49</v>
@@ -6794,7 +6795,7 @@
         <v>39</v>
       </c>
       <c r="E220">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="I220" t="s">
         <v>49</v>
@@ -6814,7 +6815,7 @@
         <v>39</v>
       </c>
       <c r="E221">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="I221" t="s">
         <v>49</v>
@@ -6834,7 +6835,7 @@
         <v>39</v>
       </c>
       <c r="E222">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="I222" t="s">
         <v>49</v>
@@ -6854,7 +6855,7 @@
         <v>39</v>
       </c>
       <c r="E223">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="I223" t="s">
         <v>49</v>
@@ -6874,7 +6875,7 @@
         <v>39</v>
       </c>
       <c r="E224">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="I224" t="s">
         <v>49</v>
@@ -6894,7 +6895,7 @@
         <v>39</v>
       </c>
       <c r="E225">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="I225" t="s">
         <v>49</v>
@@ -6914,7 +6915,7 @@
         <v>39</v>
       </c>
       <c r="E226">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I226" t="s">
         <v>49</v>
@@ -6934,7 +6935,7 @@
         <v>39</v>
       </c>
       <c r="E227">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="I227" t="s">
         <v>49</v>
@@ -6954,22 +6955,10 @@
         <v>39</v>
       </c>
       <c r="E228">
-        <v>2018</v>
-      </c>
-      <c r="G228">
-        <v>0</v>
-      </c>
-      <c r="H228" t="s">
-        <v>73</v>
+        <v>2017</v>
       </c>
       <c r="I228" t="s">
         <v>49</v>
-      </c>
-      <c r="J228" t="s">
-        <v>52</v>
-      </c>
-      <c r="L228" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.2">
@@ -6986,10 +6975,22 @@
         <v>39</v>
       </c>
       <c r="E229">
-        <v>2019</v>
+        <v>2018</v>
+      </c>
+      <c r="G229">
+        <v>0</v>
+      </c>
+      <c r="H229" t="s">
+        <v>73</v>
       </c>
       <c r="I229" t="s">
         <v>49</v>
+      </c>
+      <c r="J229" t="s">
+        <v>52</v>
+      </c>
+      <c r="L229" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.2">
@@ -7000,28 +7001,16 @@
         <v>41</v>
       </c>
       <c r="C230" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D230" t="s">
         <v>39</v>
       </c>
       <c r="E230">
-        <v>1990</v>
-      </c>
-      <c r="G230">
-        <v>0</v>
-      </c>
-      <c r="H230" t="s">
-        <v>57</v>
+        <v>2019</v>
       </c>
       <c r="I230" t="s">
         <v>49</v>
-      </c>
-      <c r="J230" t="s">
-        <v>66</v>
-      </c>
-      <c r="L230" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.2">
@@ -7038,7 +7027,7 @@
         <v>39</v>
       </c>
       <c r="E231">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G231">
         <v>0</v>
@@ -7070,7 +7059,7 @@
         <v>39</v>
       </c>
       <c r="E232">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G232">
         <v>0</v>
@@ -7102,7 +7091,7 @@
         <v>39</v>
       </c>
       <c r="E233">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G233">
         <v>0</v>
@@ -7134,7 +7123,7 @@
         <v>39</v>
       </c>
       <c r="E234">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G234">
         <v>0</v>
@@ -7166,7 +7155,7 @@
         <v>39</v>
       </c>
       <c r="E235">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G235">
         <v>0</v>
@@ -7198,7 +7187,7 @@
         <v>39</v>
       </c>
       <c r="E236">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G236">
         <v>0</v>
@@ -7230,7 +7219,7 @@
         <v>39</v>
       </c>
       <c r="E237">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G237">
         <v>0</v>
@@ -7262,7 +7251,7 @@
         <v>39</v>
       </c>
       <c r="E238">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G238">
         <v>0</v>
@@ -7294,7 +7283,7 @@
         <v>39</v>
       </c>
       <c r="E239">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G239">
         <v>0</v>
@@ -7326,7 +7315,7 @@
         <v>39</v>
       </c>
       <c r="E240">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G240">
         <v>0</v>
@@ -7358,7 +7347,7 @@
         <v>39</v>
       </c>
       <c r="E241">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G241">
         <v>0</v>
@@ -7390,7 +7379,7 @@
         <v>39</v>
       </c>
       <c r="E242">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G242">
         <v>0</v>
@@ -7422,7 +7411,7 @@
         <v>39</v>
       </c>
       <c r="E243">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G243">
         <v>0</v>
@@ -7454,7 +7443,7 @@
         <v>39</v>
       </c>
       <c r="E244">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G244">
         <v>0</v>
@@ -7486,7 +7475,7 @@
         <v>39</v>
       </c>
       <c r="E245">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G245">
         <v>0</v>
@@ -7518,7 +7507,7 @@
         <v>39</v>
       </c>
       <c r="E246">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G246">
         <v>0</v>
@@ -7550,7 +7539,7 @@
         <v>39</v>
       </c>
       <c r="E247">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G247">
         <v>0</v>
@@ -7582,7 +7571,7 @@
         <v>39</v>
       </c>
       <c r="E248">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G248">
         <v>0</v>
@@ -7614,7 +7603,7 @@
         <v>39</v>
       </c>
       <c r="E249">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G249">
         <v>0</v>
@@ -7646,7 +7635,7 @@
         <v>39</v>
       </c>
       <c r="E250">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G250">
         <v>0</v>
@@ -7678,7 +7667,7 @@
         <v>39</v>
       </c>
       <c r="E251">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G251">
         <v>0</v>
@@ -7710,7 +7699,7 @@
         <v>39</v>
       </c>
       <c r="E252">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G252">
         <v>0</v>
@@ -7742,7 +7731,7 @@
         <v>39</v>
       </c>
       <c r="E253">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G253">
         <v>0</v>
@@ -7774,7 +7763,7 @@
         <v>39</v>
       </c>
       <c r="E254">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G254">
         <v>0</v>
@@ -7806,7 +7795,7 @@
         <v>39</v>
       </c>
       <c r="E255">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G255">
         <v>0</v>
@@ -7838,7 +7827,7 @@
         <v>39</v>
       </c>
       <c r="E256">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G256">
         <v>0</v>
@@ -7870,7 +7859,7 @@
         <v>39</v>
       </c>
       <c r="E257">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G257">
         <v>0</v>
@@ -7902,7 +7891,7 @@
         <v>39</v>
       </c>
       <c r="E258">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G258">
         <v>0</v>
@@ -7934,7 +7923,7 @@
         <v>39</v>
       </c>
       <c r="E259">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G259">
         <v>0</v>
@@ -7960,28 +7949,28 @@
         <v>41</v>
       </c>
       <c r="C260" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D260" t="s">
         <v>39</v>
       </c>
       <c r="E260">
-        <v>1990</v>
+        <v>2019</v>
       </c>
       <c r="G260">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H260" t="s">
+        <v>57</v>
       </c>
       <c r="I260" t="s">
         <v>49</v>
       </c>
       <c r="J260" t="s">
-        <v>76</v>
-      </c>
-      <c r="K260" s="2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="L260" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.2">
@@ -7998,13 +7987,22 @@
         <v>39</v>
       </c>
       <c r="E261">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G261">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="I261" t="s">
         <v>49</v>
+      </c>
+      <c r="J261" t="s">
+        <v>76</v>
+      </c>
+      <c r="K261" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L261" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.2">
@@ -8021,7 +8019,7 @@
         <v>39</v>
       </c>
       <c r="E262">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G262">
         <v>0.85</v>
@@ -8044,7 +8042,7 @@
         <v>39</v>
       </c>
       <c r="E263">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G263">
         <v>0.85</v>
@@ -8067,7 +8065,7 @@
         <v>39</v>
       </c>
       <c r="E264">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G264">
         <v>0.85</v>
@@ -8090,7 +8088,7 @@
         <v>39</v>
       </c>
       <c r="E265">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G265">
         <v>0.85</v>
@@ -8113,7 +8111,7 @@
         <v>39</v>
       </c>
       <c r="E266">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G266">
         <v>0.85</v>
@@ -8136,7 +8134,7 @@
         <v>39</v>
       </c>
       <c r="E267">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G267">
         <v>0.85</v>
@@ -8159,7 +8157,7 @@
         <v>39</v>
       </c>
       <c r="E268">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G268">
         <v>0.85</v>
@@ -8182,7 +8180,7 @@
         <v>39</v>
       </c>
       <c r="E269">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G269">
         <v>0.85</v>
@@ -8205,7 +8203,7 @@
         <v>39</v>
       </c>
       <c r="E270">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G270">
         <v>0.85</v>
@@ -8228,7 +8226,7 @@
         <v>39</v>
       </c>
       <c r="E271">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G271">
         <v>0.85</v>
@@ -8251,7 +8249,7 @@
         <v>39</v>
       </c>
       <c r="E272">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G272">
         <v>0.85</v>
@@ -8274,7 +8272,7 @@
         <v>39</v>
       </c>
       <c r="E273">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G273">
         <v>0.85</v>
@@ -8297,7 +8295,7 @@
         <v>39</v>
       </c>
       <c r="E274">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G274">
         <v>0.85</v>
@@ -8320,7 +8318,7 @@
         <v>39</v>
       </c>
       <c r="E275">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G275">
         <v>0.85</v>
@@ -8343,7 +8341,7 @@
         <v>39</v>
       </c>
       <c r="E276">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G276">
         <v>0.85</v>
@@ -8366,7 +8364,7 @@
         <v>39</v>
       </c>
       <c r="E277">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G277">
         <v>0.85</v>
@@ -8389,7 +8387,7 @@
         <v>39</v>
       </c>
       <c r="E278">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G278">
         <v>0.85</v>
@@ -8412,7 +8410,7 @@
         <v>39</v>
       </c>
       <c r="E279">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G279">
         <v>0.85</v>
@@ -8435,7 +8433,7 @@
         <v>39</v>
       </c>
       <c r="E280">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G280">
         <v>0.85</v>
@@ -8458,7 +8456,7 @@
         <v>39</v>
       </c>
       <c r="E281">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G281">
         <v>0.85</v>
@@ -8481,7 +8479,7 @@
         <v>39</v>
       </c>
       <c r="E282">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G282">
         <v>0.85</v>
@@ -8504,7 +8502,7 @@
         <v>39</v>
       </c>
       <c r="E283">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G283">
         <v>0.85</v>
@@ -8527,7 +8525,7 @@
         <v>39</v>
       </c>
       <c r="E284">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G284">
         <v>0.85</v>
@@ -8550,7 +8548,7 @@
         <v>39</v>
       </c>
       <c r="E285">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G285">
         <v>0.85</v>
@@ -8573,7 +8571,7 @@
         <v>39</v>
       </c>
       <c r="E286">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G286">
         <v>0.85</v>
@@ -8596,7 +8594,7 @@
         <v>39</v>
       </c>
       <c r="E287">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G287">
         <v>0.85</v>
@@ -8619,7 +8617,7 @@
         <v>39</v>
       </c>
       <c r="E288">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G288">
         <v>0.85</v>
@@ -8642,7 +8640,7 @@
         <v>39</v>
       </c>
       <c r="E289">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G289">
         <v>0.85</v>
@@ -8659,16 +8657,16 @@
         <v>41</v>
       </c>
       <c r="C290" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D290" t="s">
         <v>39</v>
       </c>
       <c r="E290">
-        <v>1990</v>
+        <v>2019</v>
       </c>
       <c r="G290">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="I290" t="s">
         <v>49</v>
@@ -8688,10 +8686,10 @@
         <v>39</v>
       </c>
       <c r="E291">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G291">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I291" t="s">
         <v>49</v>
@@ -8711,7 +8709,7 @@
         <v>39</v>
       </c>
       <c r="E292">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G292">
         <v>0.1</v>
@@ -8734,7 +8732,7 @@
         <v>39</v>
       </c>
       <c r="E293">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G293">
         <v>0.1</v>
@@ -8757,7 +8755,7 @@
         <v>39</v>
       </c>
       <c r="E294">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G294">
         <v>0.1</v>
@@ -8780,7 +8778,7 @@
         <v>39</v>
       </c>
       <c r="E295">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G295">
         <v>0.1</v>
@@ -8803,7 +8801,7 @@
         <v>39</v>
       </c>
       <c r="E296">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G296">
         <v>0.1</v>
@@ -8826,7 +8824,7 @@
         <v>39</v>
       </c>
       <c r="E297">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G297">
         <v>0.1</v>
@@ -8849,7 +8847,7 @@
         <v>39</v>
       </c>
       <c r="E298">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G298">
         <v>0.1</v>
@@ -8872,7 +8870,7 @@
         <v>39</v>
       </c>
       <c r="E299">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G299">
         <v>0.1</v>
@@ -8895,7 +8893,7 @@
         <v>39</v>
       </c>
       <c r="E300">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G300">
         <v>0.1</v>
@@ -8918,7 +8916,7 @@
         <v>39</v>
       </c>
       <c r="E301">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G301">
         <v>0.1</v>
@@ -8941,7 +8939,7 @@
         <v>39</v>
       </c>
       <c r="E302">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G302">
         <v>0.1</v>
@@ -8964,7 +8962,7 @@
         <v>39</v>
       </c>
       <c r="E303">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G303">
         <v>0.1</v>
@@ -8987,7 +8985,7 @@
         <v>39</v>
       </c>
       <c r="E304">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G304">
         <v>0.1</v>
@@ -9010,7 +9008,7 @@
         <v>39</v>
       </c>
       <c r="E305">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G305">
         <v>0.1</v>
@@ -9033,7 +9031,7 @@
         <v>39</v>
       </c>
       <c r="E306">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G306">
         <v>0.1</v>
@@ -9056,7 +9054,7 @@
         <v>39</v>
       </c>
       <c r="E307">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G307">
         <v>0.1</v>
@@ -9079,7 +9077,7 @@
         <v>39</v>
       </c>
       <c r="E308">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G308">
         <v>0.1</v>
@@ -9102,7 +9100,7 @@
         <v>39</v>
       </c>
       <c r="E309">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G309">
         <v>0.1</v>
@@ -9125,7 +9123,7 @@
         <v>39</v>
       </c>
       <c r="E310">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G310">
         <v>0.1</v>
@@ -9148,7 +9146,7 @@
         <v>39</v>
       </c>
       <c r="E311">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G311">
         <v>0.1</v>
@@ -9171,7 +9169,7 @@
         <v>39</v>
       </c>
       <c r="E312">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G312">
         <v>0.1</v>
@@ -9194,7 +9192,7 @@
         <v>39</v>
       </c>
       <c r="E313">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G313">
         <v>0.1</v>
@@ -9217,7 +9215,7 @@
         <v>39</v>
       </c>
       <c r="E314">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G314">
         <v>0.1</v>
@@ -9240,7 +9238,7 @@
         <v>39</v>
       </c>
       <c r="E315">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G315">
         <v>0.1</v>
@@ -9263,7 +9261,7 @@
         <v>39</v>
       </c>
       <c r="E316">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G316">
         <v>0.1</v>
@@ -9286,7 +9284,7 @@
         <v>39</v>
       </c>
       <c r="E317">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G317">
         <v>0.1</v>
@@ -9309,7 +9307,7 @@
         <v>39</v>
       </c>
       <c r="E318">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G318">
         <v>0.1</v>
@@ -9332,7 +9330,7 @@
         <v>39</v>
       </c>
       <c r="E319">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G319">
         <v>0.1</v>
@@ -9341,14 +9339,37 @@
         <v>49</v>
       </c>
     </row>
-    <row r="432" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K432" s="2"/>
+    <row r="320" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A320" t="s">
+        <v>16</v>
+      </c>
+      <c r="B320" t="s">
+        <v>41</v>
+      </c>
+      <c r="C320" t="s">
+        <v>29</v>
+      </c>
+      <c r="D320" t="s">
+        <v>39</v>
+      </c>
+      <c r="E320">
+        <v>2019</v>
+      </c>
+      <c r="G320">
+        <v>0.1</v>
+      </c>
+      <c r="I320" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="433" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K433" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:L852" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A5:L853" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K260" r:id="rId1" xr:uid="{F4373F22-5F19-834C-83D0-AE7B39FD63BE}"/>
+    <hyperlink ref="K261" r:id="rId1" xr:uid="{F4373F22-5F19-834C-83D0-AE7B39FD63BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Zenodo files (electricity)
</commit_message>
<xml_diff>
--- a/data/zenodo/conversion/chp/CHE_convchp_biogas.xlsx
+++ b/data/zenodo/conversion/chp/CHE_convchp_biogas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/zenodo/conversion/chp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F5C673-0065-3D45-BFFB-78DB02C8C299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC93B14D-5E85-9841-82FC-F60D0A245871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -395,9 +395,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -435,9 +435,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -470,26 +470,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -522,26 +505,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -718,8 +684,8 @@
   <dimension ref="A1:L433"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <pane ySplit="5" topLeftCell="A258" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I265" sqref="I265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7990,7 +7956,7 @@
         <v>1990</v>
       </c>
       <c r="G261">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="I261" t="s">
         <v>49</v>
@@ -8689,7 +8655,7 @@
         <v>1990</v>
       </c>
       <c r="G291">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I291" t="s">
         <v>49</v>

</xml_diff>